<commit_message>
SMILES autoencoders & morgan bits
</commit_message>
<xml_diff>
--- a/Molecules-data/smiles_prop_3xtr_WithTokenMol.xlsx
+++ b/Molecules-data/smiles_prop_3xtr_WithTokenMol.xlsx
@@ -37,140 +37,143 @@
     <t>pixels</t>
   </si>
   <si>
-    <t>O=C(Nc1cccc2ccccc12)c1cc2cc(Cl)ccc2oc1=O</t>
-  </si>
-  <si>
-    <t>['O', '=', 'C', '(', 'N', 'c', '1', 'c', 'c', 'c', 'c', '2', 'c', 'c', 'c', 'c', 'c', '1', '2', ')', 'c', '1', 'c', 'c', '2', 'c', 'c', '(', 'Cl', ')', 'c', 'c', 'c', '2', 'o', 'c', '1', '=', 'O']</t>
+    <t>CCOC(=O)C1=C(C)NC(=S)N[C@H]1c1cccc([N+](=O)[O-])c1</t>
+  </si>
+  <si>
+    <t>['C', 'C', 'O', 'C', '(', '=', 'O', ')', 'C', '1', '=', 'C', '(', 'C', ')', 'N', 'C', '(', '=', 'S', ')', 'N', '[C@H]', '1', 'c', '1', 'c', 'c', 'c', 'c', '(', '[N+]', '(', '=', 'O', ')', '[O-]', ')', 'c', '1']</t>
   </si>
   <si>
     <t>[[1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
  [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
  [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
  [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
  [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
  [0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
  [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 1 0 0 0 0 0 0]
  [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
  [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
  [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 1 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 1 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 1 0 0 0 0 0 0 0 0]]</t>
+  </si>
+  <si>
+    <t>COC(=O)c1ccccc1OC(=O)C(C)C</t>
+  </si>
+  <si>
+    <t>['C', 'O', 'C', '(', '=', 'O', ')', 'c', '1', 'c', 'c', 'c', 'c', 'c', '1', 'O', 'C', '(', '=', 'O', ')', 'C', '(', 'C', ')', 'C']</t>
+  </si>
+  <si>
+    <t>[[1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
  [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 1 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
  [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
  [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 1 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0]]</t>
-  </si>
-  <si>
-    <t>CC(C)Cc1ccc(S(=O)(=O)N2CCCc3ccccc32)cc1</t>
-  </si>
-  <si>
-    <t>['C', 'C', '(', 'C', ')', 'C', 'c', '1', 'c', 'c', 'c', '(', 'S', '(', '=', 'O', ')', '(', '=', 'O', ')', 'N', '2', 'C', 'C', 'C', 'c', '3', 'c', 'c', 'c', 'c', 'c', '3', '2', ')', 'c', 'c', '1']</t>
-  </si>
-  <si>
-    <t>[[0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]]</t>
+  </si>
+  <si>
+    <t>CCCc1nc(SCC(=O)N2CCOCC2)c2ccccc2n1</t>
+  </si>
+  <si>
+    <t>['C', 'C', 'C', 'c', '1', 'n', 'c', '(', 'S', 'C', 'C', '(', '=', 'O', ')', 'N', '2', 'C', 'C', 'O', 'C', 'C', '2', ')', 'c', '2', 'c', 'c', 'c', 'c', 'c', '2', 'n', '1']</t>
+  </si>
+  <si>
+    <t>[[1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
  [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
  [0 0 0 0 0 0 0 0 0 0 0 0 1 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 1 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 1]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 1]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 1]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 1]
+ [0 0 0 0 0 0 0 0 0 0 0 0 1 0]
  [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 1 0]
- [0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0]]</t>
-  </si>
-  <si>
-    <t>CNC(=O)/C(=C/c1ccco1)NC(=O)c1ccco1</t>
-  </si>
-  <si>
-    <t>['C', 'N', 'C', '(', '=', 'O', ')', '/', 'C', '(', '=', 'C', '/', 'c', '1', 'c', 'c', 'c', 'o', '1', ')', 'N', 'C', '(', '=', 'O', ')', 'c', '1', 'c', 'c', 'c', 'o', '1']</t>
-  </si>
-  <si>
-    <t>[[0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 1]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 1]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 1 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 1 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
  [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
  [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
  [0 0 0 0 0 0 0 0 0 0 0 0 0 0]
@@ -663,13 +666,13 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>349.050570924</v>
+        <v>321.07832696</v>
       </c>
       <c r="D2">
-        <v>4.8519</v>
+        <v>1.9507</v>
       </c>
       <c r="E2">
-        <v>59.31</v>
+        <v>93.5</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -686,13 +689,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>329.144949976</v>
+        <v>222.089208928</v>
       </c>
       <c r="D3">
-        <v>4.0266</v>
+        <v>2.0346</v>
       </c>
       <c r="E3">
-        <v>37.38</v>
+        <v>52.6</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -709,13 +712,13 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>260.079706864</v>
+        <v>331.135447912</v>
       </c>
       <c r="D4">
-        <v>1.3895</v>
+        <v>2.5332</v>
       </c>
       <c r="E4">
-        <v>84.48</v>
+        <v>55.32</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
iris4 is working again
</commit_message>
<xml_diff>
--- a/Molecules-data/smiles_prop_3xtr_WithTokenMol.xlsx
+++ b/Molecules-data/smiles_prop_3xtr_WithTokenMol.xlsx
@@ -40,175 +40,184 @@
     <t>ROMol</t>
   </si>
   <si>
-    <t>COC(=O)c1ccc(/C=c2\sc3nc(-c4ccc(C)cc4)nn3c2=O)cc1</t>
-  </si>
-  <si>
-    <t>['C', 'O', 'C', '(', '=', 'O', ')', 'c', '1', 'c', 'c', 'c', '(', '/', 'C', '=', 'c', '2', '\\', 's', 'c', '3', 'n', 'c', '(', '-', 'c', '4', 'c', 'c', 'c', '(', 'C', ')', 'c', 'c', '4', ')', 'n', 'n', '3', 'c', '2', '=', 'O', ')', 'c', 'c', '1']</t>
-  </si>
-  <si>
-    <t>[[1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]]</t>
-  </si>
-  <si>
-    <t>CCOc1ccc(C(=O)Nc2cccc(-c3nc4ncccc4o3)c2C)cc1</t>
-  </si>
-  <si>
-    <t>['C', 'C', 'O', 'c', '1', 'c', 'c', 'c', '(', 'C', '(', '=', 'O', ')', 'N', 'c', '2', 'c', 'c', 'c', 'c', '(', '-', 'c', '3', 'n', 'c', '4', 'n', 'c', 'c', 'c', 'c', '4', 'o', '3', ')', 'c', '2', 'C', ')', 'c', 'c', '1']</t>
-  </si>
-  <si>
-    <t>[[1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]]</t>
-  </si>
-  <si>
-    <t>Cc1ccc(C(=O)C[C@]2(O)C(=O)N(CCc3ccccc3)c3ccccc32)cc1</t>
-  </si>
-  <si>
-    <t>['C', 'c', '1', 'c', 'c', 'c', '(', 'C', '(', '=', 'O', ')', 'C', '[C@]', '2', '(', 'O', ')', 'C', '(', '=', 'O', ')', 'N', '(', 'C', 'C', 'c', '3', 'c', 'c', 'c', 'c', 'c', '3', ')', 'c', '3', 'c', 'c', 'c', 'c', 'c', '3', '2', ')', 'c', 'c', '1']</t>
-  </si>
-  <si>
-    <t>[[1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0]
- [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
- [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
- [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]]</t>
+    <t>O=Cc1cc2cccc3c2n(c1=O)CCC3</t>
+  </si>
+  <si>
+    <t>['O', '=', 'C', 'c', '1', 'c', 'c', '2', 'c', 'c', 'c', 'c', '3', 'c', '2', 'n', '(', 'c', '1', '=', 'O', ')', 'C', 'C', 'C', '3']</t>
+  </si>
+  <si>
+    <t>[[1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]]</t>
+  </si>
+  <si>
+    <t>CC(C)(C)[C@H]1CCc2c(sc(NC(=O)c3ccc4c(c3)OCO4)c2C(N)=O)C1</t>
+  </si>
+  <si>
+    <t>['C', 'C', '(', 'C', ')', '(', 'C', ')', '[C@H]', '1', 'C', 'C', 'c', '2', 'c', '(', 's', 'c', '(', 'N', 'C', '(', '=', 'O', ')', 'c', '3', 'c', 'c', 'c', '4', 'c', '(', 'c', '3', ')', 'O', 'C', 'O', '4', ')', 'c', '2', 'C', '(', 'N', ')', '=', 'O', ')', 'C', '1']</t>
+  </si>
+  <si>
+    <t>[[0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]]</t>
+  </si>
+  <si>
+    <t>Cc1ccc(S[C@@H](C)C(=O)Nc2cccc(C(F)(F)F)c2)cc1</t>
+  </si>
+  <si>
+    <t>['C', 'c', '1', 'c', 'c', 'c', '(', 'S', '[C@@H]', '(', 'C', ')', 'C', '(', '=', 'O', ')', 'N', 'c', '2', 'c', 'c', 'c', 'c', '(', 'C', '(', 'F', ')', '(', 'F', ')', 'F', ')', 'c', '2', ')', 'c', 'c', '1']</t>
+  </si>
+  <si>
+    <t>[[0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]
+ [0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0]]</t>
   </si>
 </sst>
 </file>
@@ -699,13 +708,13 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>377.08341234</v>
+        <v>213.078978592</v>
       </c>
       <c r="C2">
-        <v>2.46072</v>
+        <v>1.7602</v>
       </c>
       <c r="D2">
-        <v>73.56</v>
+        <v>39.07</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -722,13 +731,13 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>373.142641468</v>
+        <v>400.145678248</v>
       </c>
       <c r="C3">
-        <v>4.84922</v>
+        <v>3.979</v>
       </c>
       <c r="D3">
-        <v>77.25</v>
+        <v>90.65000000000001</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -745,13 +754,13 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>385.167793596</v>
+        <v>339.090469792</v>
       </c>
       <c r="C4">
-        <v>4.04492</v>
+        <v>5.13312</v>
       </c>
       <c r="D4">
-        <v>57.61</v>
+        <v>29.1</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>

</xml_diff>